<commit_message>
scenario r002 - modifications on coordinates
scenario doesn't run, but network is generated
</commit_message>
<xml_diff>
--- a/scenarios/01_original_data/hubs_distances.xlsx
+++ b/scenarios/01_original_data/hubs_distances.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
-  <si>
-    <t>gossau</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>genève la praille</t>
   </si>
@@ -222,9 +219,6 @@
     <t>zimeysa-meyrin</t>
   </si>
   <si>
-    <t>;genève la praille;val ombré;genève aéroport;nyon;gland;aubonne;tolochenaz-morges;léman;aclens;daillens;chavorney;yverdon;payerne;avanches;broye;kerzers;lyss ort;solothurn-zuchwil;niederbipp;neuendorf;härkingen;rickenbach-wangen;dulliken süd;suhr;schafisheim;heitersberg;urdorf;zürich aussersihl;zürich nord;zürich flughafen;aegert;winterthur;winterthur hegi;frauenfeld;wil;uzwil-oberbüren;gossau;st. gallen st. fiden;oftringen-zofingen;dagmersellen;sursee;rothenburg;emmenbrücke;luzern allmend;dulliken;sissach;liestal;mayenfels;basel wolf;basel gateway nord;lyss;biel/bienne;pratteln west;limmatstadt;wangen-dübendorf;schönbühl;bern;bern wankdorf;muri-gümligen;münsingen;heimberg-steffisburg;gwatt;bern weyermannshaus;fribourg;crissier;lausanne-malley;zimeysa-meyrin</t>
-  </si>
-  <si>
     <t>genève la praille;;10.6;15.8;51.4;61.4;87;101.2;119.2;122.4;137.8;156.6;173;221.6;247;273.2;301.4;334.2;381.2;409.2;424.8;428.8;437.84;451.22;475.96;483.54;519.36;532.56;546.76;559.76;572.76;578.16;607.56;613.76;640.76;673.96;695.96;720.96;738.76;460.42;484.42;505.22;535.02;541.62;550.02;454.22;488.62;502.62;510.74;526.04;538.04;337.8;355.1;513.34;523.56;582.36;364.2;376.2;386.1;397.06;414.22;436.22;454.9;386.2;309.2;125.2;133.3;15.4</t>
   </si>
   <si>
@@ -333,9 +327,6 @@
     <t>uzwil-oberbüren;695.96;685.36;680.16;644.56;634.56;608.96;594.76;576.76;573.56;558.16;539.36;522.96;474.36;448.96;422.76;394.56;361.76;314.76;286.76;271.16;267.16;258.12;244.74;220;212.42;176.6;163.4;149.2;136.2;123.2;117.8;88.4;82.2;55.2;22;;25;42.8;253.94;277.94;298.74;328.54;335.14;343.54;247.74;282.14;296.14;304.26;319.56;331.56;365.36;382.66;306.86;180.8;122;391.76;403.76;413.66;424.62;441.78;463.78;482.46;413.76;458.76;582.76;590.86;690.16</t>
   </si>
   <si>
-    <t>gossau;720.96;710.36;705.16;669.56;659.56;633.96;619.76;601.76;598.56;583.16;564.36;547.96;499.36;473.96;447.76;419.56;386.76;339.76;311.76;296.16;292.16;283.12;269.74;245;237.42;201.6;188.4;174.2;161.2;148.2;142.8;113.4;107.2;80.2;47;25;;17.8;278.94;302.94;323.74;353.54;360.14;368.54;272.74;307.14;321.14;329.26;344.56;356.56;390.36;407.66;331.86;205.8;147;416.76;428.76;438.66;449.62;466.78;488.78;507.46;438.76;483.76;607.76;615.86;715.16</t>
-  </si>
-  <si>
     <t>st. gallen st. fiden;738.76;728.16;722.96;687.36;677.36;651.76;637.56;619.56;616.36;600.96;582.16;565.76;517.16;491.76;465.56;437.36;404.56;357.56;329.56;313.96;309.96;300.92;287.54;262.8;255.22;219.4;206.2;192;179;166;160.6;131.2;125;98;64.8;42.8;17.8;;296.74;320.74;341.54;371.34;377.94;386.34;290.54;324.94;338.94;347.06;362.36;374.36;408.16;425.46;349.66;223.6;164.8;434.56;446.56;456.46;467.42;484.58;506.58;525.26;456.56;501.56;625.56;633.66;732.96</t>
   </si>
   <si>
@@ -424,6 +415,12 @@
   </si>
   <si>
     <t>zimeysa-meyrin;15.4;4.8;10;45.6;55.6;81.2;95.4;113.4;116.6;132;150.8;167.2;215.8;241.2;267.4;295.6;328.4;375.4;403.4;419;423;432.04;445.42;470.16;477.74;513.56;526.76;540.96;553.96;566.96;572.36;601.76;607.96;634.96;668.16;690.16;715.16;732.96;454.62;478.62;499.42;529.22;535.82;544.22;448.42;482.82;496.82;504.94;520.24;532.24;332;349.3;507.54;517.76;576.56;358.4;370.4;380.3;391.26;408.42;430.42;449.1;380.4;303.4;119.4;127.5;</t>
+  </si>
+  <si>
+    <t>gossaucst</t>
+  </si>
+  <si>
+    <t>gossaucst;720.96;710.36;705.16;669.56;659.56;633.96;619.76;601.76;598.56;583.16;564.36;547.96;499.36;473.96;447.76;419.56;386.76;339.76;311.76;296.16;292.16;283.12;269.74;245;237.42;201.6;188.4;174.2;161.2;148.2;142.8;113.4;107.2;80.2;47;25;;17.8;278.94;302.94;323.74;353.54;360.14;368.54;272.74;307.14;321.14;329.26;344.56;356.56;390.36;407.66;331.86;205.8;147;416.76;428.76;438.66;449.62;466.78;488.78;507.46;438.76;483.76;607.76;615.86;715.16</t>
   </si>
 </sst>
 </file>
@@ -1232,225 +1229,220 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BS11" sqref="BS11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>67</v>
-      </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>65</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>66</v>
       </c>
       <c r="BT1" t="str">
         <f>CONCATENATE(A1,";",B1,";",C1,";",D1,";",E1,";",F1,";",G1,";",H1,";",I1,";",J1,";",K1,";",L1,";",M1,";",N1,";",O1,";",P1,";",Q1,";",R1,";",S1,";",T1,";",U1,";",V1,";",W1,";",X1,";",Y1,";",Z1,";",AA1,";",AB1,";",AC1,";",AD1,";",AE1,";",AF1,";",AG1,";",AH1,";",AI1,";",AJ1,";",AK1,";",AL1,";",AM1,";",AN1,";",AO1,";",AP1,";",AQ1,";",AR1,";",AS1,";",AT1,";",AU1,";",AV1,";",AW1,";",AX1,";",AY1,";",AZ1,";",BA1,";",BB1,";",BC1,";",BD1,";",BE1,";",BF1,";",BG1,";",BH1,";",BI1,";",BJ1,";",BK1,";",BL1,";",BM1,";",BN1,";",BO1,";",BP1)</f>
-        <v>;genève la praille;val ombré;genève aéroport;nyon;gland;aubonne;tolochenaz-morges;léman;aclens;daillens;chavorney;yverdon;payerne;avanches;broye;kerzers;lyss ort;solothurn-zuchwil;niederbipp;neuendorf;härkingen;rickenbach-wangen;dulliken süd;suhr;schafisheim;heitersberg;urdorf;zürich aussersihl;zürich nord;zürich flughafen;aegert;winterthur;winterthur hegi;frauenfeld;wil;uzwil-oberbüren;gossau;st. gallen st. fiden;oftringen-zofingen;dagmersellen;sursee;rothenburg;emmenbrücke;luzern allmend;dulliken;sissach;liestal;mayenfels;basel wolf;basel gateway nord;lyss;biel/bienne;pratteln west;limmatstadt;wangen-dübendorf;schönbühl;bern;bern wankdorf;muri-gümligen;münsingen;heimberg-steffisburg;gwatt;bern weyermannshaus;fribourg;crissier;lausanne-malley;zimeysa-meyrin;genève la praille;val ombré;genève aéroport;nyon;gland;aubonne;tolochenaz-morges;léman;aclens;daillens;chavorney;yverdon;payerne;avanches;broye;kerzers;lyss ort;solothurn-zuchwil;niederbipp;neuendorf;härkingen;rickenbach-wangen;dulliken süd;suhr;schafisheim;heitersberg;urdorf;zürich aussersihl;zürich nord;zürich flughafen;aegert;winterthur;winterthur hegi;frauenfeld;wil;uzwil-oberbüren;gossau;st. gallen st. fiden;oftringen-zofingen;dagmersellen;sursee;rothenburg;emmenbrücke;luzern allmend;dulliken;sissach;liestal;mayenfels;basel wolf;basel gateway nord;lyss;biel/bienne;pratteln west;limmatstadt;wangen-dübendorf;schönbühl;bern;bern wankdorf;muri-gümligen;münsingen;heimberg-steffisburg;gwatt;bern weyermannshaus;fribourg;crissier;lausanne-malley;zimeysa-meyrin</v>
+        <v>;genève la praille;val ombré;genève aéroport;nyon;gland;aubonne;tolochenaz-morges;léman;aclens;daillens;chavorney;yverdon;payerne;avanches;broye;kerzers;lyss ort;solothurn-zuchwil;niederbipp;neuendorf;härkingen;rickenbach-wangen;dulliken süd;suhr;schafisheim;heitersberg;urdorf;zürich aussersihl;zürich nord;zürich flughafen;aegert;winterthur;winterthur hegi;frauenfeld;wil;uzwil-oberbüren;gossaucst;st. gallen st. fiden;oftringen-zofingen;dagmersellen;sursee;rothenburg;emmenbrücke;luzern allmend;dulliken;sissach;liestal;mayenfels;basel wolf;basel gateway nord;lyss;biel/bienne;pratteln west;limmatstadt;wangen-dübendorf;schönbühl;bern;bern wankdorf;muri-gümligen;münsingen;heimberg-steffisburg;gwatt;bern weyermannshaus;fribourg;crissier;lausanne-malley;zimeysa-meyrin</v>
       </c>
     </row>
     <row r="2" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2">
         <v>10.6</v>
@@ -1657,7 +1649,7 @@
     </row>
     <row r="3" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>10.6</v>
@@ -1864,7 +1856,7 @@
     </row>
     <row r="4" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>15.8</v>
@@ -2071,7 +2063,7 @@
     </row>
     <row r="5" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5">
         <v>51.4</v>
@@ -2278,7 +2270,7 @@
     </row>
     <row r="6" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6">
         <v>61.399999999999991</v>
@@ -2485,7 +2477,7 @@
     </row>
     <row r="7" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <v>87</v>
@@ -2692,7 +2684,7 @@
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>101.2</v>
@@ -2899,7 +2891,7 @@
     </row>
     <row r="9" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>119.2</v>
@@ -3106,7 +3098,7 @@
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>122.4</v>
@@ -3313,7 +3305,7 @@
     </row>
     <row r="11" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11">
         <v>137.80000000000001</v>
@@ -3520,7 +3512,7 @@
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12">
         <v>156.6</v>
@@ -3727,7 +3719,7 @@
     </row>
     <row r="13" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13">
         <v>173</v>
@@ -3934,7 +3926,7 @@
     </row>
     <row r="14" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B14">
         <v>221.6</v>
@@ -4141,7 +4133,7 @@
     </row>
     <row r="15" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B15">
         <v>247</v>
@@ -4348,7 +4340,7 @@
     </row>
     <row r="16" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B16">
         <v>273.2</v>
@@ -4555,7 +4547,7 @@
     </row>
     <row r="17" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17">
         <v>301.39999999999998</v>
@@ -4762,7 +4754,7 @@
     </row>
     <row r="18" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18">
         <v>334.2</v>
@@ -4969,7 +4961,7 @@
     </row>
     <row r="19" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19">
         <v>381.2</v>
@@ -5176,7 +5168,7 @@
     </row>
     <row r="20" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B20">
         <v>409.2</v>
@@ -5383,7 +5375,7 @@
     </row>
     <row r="21" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21">
         <v>424.8</v>
@@ -5590,7 +5582,7 @@
     </row>
     <row r="22" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22">
         <v>428.8</v>
@@ -5797,7 +5789,7 @@
     </row>
     <row r="23" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23">
         <v>437.84</v>
@@ -6004,7 +5996,7 @@
     </row>
     <row r="24" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24">
         <v>451.22</v>
@@ -6211,7 +6203,7 @@
     </row>
     <row r="25" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B25">
         <v>475.96</v>
@@ -6418,7 +6410,7 @@
     </row>
     <row r="26" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26">
         <v>483.54</v>
@@ -6625,7 +6617,7 @@
     </row>
     <row r="27" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27">
         <v>519.36</v>
@@ -6832,7 +6824,7 @@
     </row>
     <row r="28" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28">
         <v>532.55999999999995</v>
@@ -7039,7 +7031,7 @@
     </row>
     <row r="29" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B29">
         <v>546.76</v>
@@ -7246,7 +7238,7 @@
     </row>
     <row r="30" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B30">
         <v>559.76</v>
@@ -7453,7 +7445,7 @@
     </row>
     <row r="31" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B31">
         <v>572.76</v>
@@ -7660,7 +7652,7 @@
     </row>
     <row r="32" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B32">
         <v>578.16</v>
@@ -7867,7 +7859,7 @@
     </row>
     <row r="33" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B33">
         <v>607.55999999999995</v>
@@ -8074,7 +8066,7 @@
     </row>
     <row r="34" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B34">
         <v>613.76</v>
@@ -8281,7 +8273,7 @@
     </row>
     <row r="35" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B35">
         <v>640.76</v>
@@ -8488,7 +8480,7 @@
     </row>
     <row r="36" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B36">
         <v>673.95999999999992</v>
@@ -8695,7 +8687,7 @@
     </row>
     <row r="37" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B37">
         <v>695.95999999999992</v>
@@ -8902,7 +8894,7 @@
     </row>
     <row r="38" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="B38">
         <v>720.95999999999992</v>
@@ -9104,12 +9096,12 @@
       </c>
       <c r="BT38" t="str">
         <f t="shared" si="0"/>
-        <v>gossau;720.96;710.36;705.16;669.56;659.56;633.96;619.76;601.76;598.56;583.16;564.36;547.96;499.36;473.96;447.76;419.56;386.76;339.76;311.76;296.16;292.16;283.12;269.74;245;237.42;201.6;188.4;174.2;161.2;148.2;142.8;113.4;107.2;80.2;47;25;;17.8;278.94;302.94;323.74;353.54;360.14;368.54;272.74;307.14;321.14;329.26;344.56;356.56;390.36;407.66;331.86;205.8;147;416.76;428.76;438.66;449.62;466.78;488.78;507.46;438.76;483.76;607.76;615.86;715.16;720.96;710.36;705.16;669.56;659.56;633.96;619.76;601.76;598.56;583.16;564.36;547.96;499.36;473.96;447.76;419.56;386.76;339.76;311.76;296.16;292.16;283.12;269.74;245;237.42;201.6;188.4;174.2;161.2;148.2;142.8;113.4;107.2;80.2;47;25;;17.8;278.94;302.94;323.74;353.54;360.14;368.54;272.74;307.14;321.14;329.26;344.56;356.56;390.36;407.66;331.86;205.8;147;416.76;428.76;438.66;449.62;466.78;488.78;507.46;438.76;483.76;607.76;615.86;715.16</v>
+        <v>gossaucst;720.96;710.36;705.16;669.56;659.56;633.96;619.76;601.76;598.56;583.16;564.36;547.96;499.36;473.96;447.76;419.56;386.76;339.76;311.76;296.16;292.16;283.12;269.74;245;237.42;201.6;188.4;174.2;161.2;148.2;142.8;113.4;107.2;80.2;47;25;;17.8;278.94;302.94;323.74;353.54;360.14;368.54;272.74;307.14;321.14;329.26;344.56;356.56;390.36;407.66;331.86;205.8;147;416.76;428.76;438.66;449.62;466.78;488.78;507.46;438.76;483.76;607.76;615.86;715.16;720.96;710.36;705.16;669.56;659.56;633.96;619.76;601.76;598.56;583.16;564.36;547.96;499.36;473.96;447.76;419.56;386.76;339.76;311.76;296.16;292.16;283.12;269.74;245;237.42;201.6;188.4;174.2;161.2;148.2;142.8;113.4;107.2;80.2;47;25;;17.8;278.94;302.94;323.74;353.54;360.14;368.54;272.74;307.14;321.14;329.26;344.56;356.56;390.36;407.66;331.86;205.8;147;416.76;428.76;438.66;449.62;466.78;488.78;507.46;438.76;483.76;607.76;615.86;715.16</v>
       </c>
     </row>
     <row r="39" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B39">
         <v>738.76</v>
@@ -9316,7 +9308,7 @@
     </row>
     <row r="40" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B40">
         <v>460.42</v>
@@ -9523,7 +9515,7 @@
     </row>
     <row r="41" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B41">
         <v>484.42</v>
@@ -9730,7 +9722,7 @@
     </row>
     <row r="42" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B42">
         <v>505.22</v>
@@ -9937,7 +9929,7 @@
     </row>
     <row r="43" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B43">
         <v>535.02</v>
@@ -10144,7 +10136,7 @@
     </row>
     <row r="44" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B44">
         <v>541.62</v>
@@ -10351,7 +10343,7 @@
     </row>
     <row r="45" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B45">
         <v>550.02</v>
@@ -10558,7 +10550,7 @@
     </row>
     <row r="46" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B46">
         <v>454.22</v>
@@ -10765,7 +10757,7 @@
     </row>
     <row r="47" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B47">
         <v>488.61999999999989</v>
@@ -10972,7 +10964,7 @@
     </row>
     <row r="48" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B48">
         <v>502.61999999999989</v>
@@ -11179,7 +11171,7 @@
     </row>
     <row r="49" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B49">
         <v>510.74</v>
@@ -11386,7 +11378,7 @@
     </row>
     <row r="50" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B50">
         <v>526.04</v>
@@ -11593,7 +11585,7 @@
     </row>
     <row r="51" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B51">
         <v>538.04</v>
@@ -11800,7 +11792,7 @@
     </row>
     <row r="52" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B52">
         <v>337.8</v>
@@ -12007,7 +11999,7 @@
     </row>
     <row r="53" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B53">
         <v>355.1</v>
@@ -12214,7 +12206,7 @@
     </row>
     <row r="54" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B54">
         <v>513.33999999999992</v>
@@ -12421,7 +12413,7 @@
     </row>
     <row r="55" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B55">
         <v>523.55999999999995</v>
@@ -12628,7 +12620,7 @@
     </row>
     <row r="56" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B56">
         <v>582.36</v>
@@ -12835,7 +12827,7 @@
     </row>
     <row r="57" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B57">
         <v>364.2</v>
@@ -13042,7 +13034,7 @@
     </row>
     <row r="58" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B58">
         <v>376.2</v>
@@ -13249,7 +13241,7 @@
     </row>
     <row r="59" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B59">
         <v>386.1</v>
@@ -13456,7 +13448,7 @@
     </row>
     <row r="60" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B60">
         <v>397.06</v>
@@ -13663,7 +13655,7 @@
     </row>
     <row r="61" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B61">
         <v>414.22</v>
@@ -13870,7 +13862,7 @@
     </row>
     <row r="62" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B62">
         <v>436.22</v>
@@ -14077,7 +14069,7 @@
     </row>
     <row r="63" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B63">
         <v>454.89999999999992</v>
@@ -14284,7 +14276,7 @@
     </row>
     <row r="64" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B64">
         <v>386.2</v>
@@ -14491,7 +14483,7 @@
     </row>
     <row r="65" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B65">
         <v>309.2</v>
@@ -14698,7 +14690,7 @@
     </row>
     <row r="66" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B66">
         <v>125.2</v>
@@ -14905,7 +14897,7 @@
     </row>
     <row r="67" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B67">
         <v>133.30000000000001</v>
@@ -15112,7 +15104,7 @@
     </row>
     <row r="68" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B68">
         <v>15.4</v>

</xml_diff>